<commit_message>
fix(*):Fix priority of volume - fix some bugs
</commit_message>
<xml_diff>
--- a/docs/日程安排.xlsx
+++ b/docs/日程安排.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\47126\Desktop\Migrate策划案\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Unity Project\Migrate\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E9A8E9B-DC32-4E78-8019-AB9F8A52E993}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C6E81FB-AA85-4A58-9AB4-049E08973574}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="76">
   <si>
     <t>周次</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -324,6 +324,10 @@
   <si>
     <t>事件系统全部完成,缺少配图
 完善场景</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>时间模块</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -362,7 +366,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -443,12 +447,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -630,7 +628,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -705,9 +703,6 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -717,13 +712,13 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="58" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -747,6 +742,132 @@
     <xf numFmtId="58" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -774,27 +895,6 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -803,111 +903,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1198,8 +1193,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23:D29"/>
+    <sheetView tabSelected="1" topLeftCell="B58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H65" sqref="H65:H71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1245,7 +1240,7 @@
       <c r="J1" s="7"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="47" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="19">
@@ -1254,132 +1249,132 @@
       <c r="C2" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="58"/>
-      <c r="E2" s="54" t="s">
+      <c r="D2" s="92"/>
+      <c r="E2" s="78" t="s">
         <v>40</v>
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="61"/>
-      <c r="I2" s="64" t="s">
+      <c r="H2" s="71"/>
+      <c r="I2" s="74" t="s">
         <v>39</v>
       </c>
       <c r="J2" s="7"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="52"/>
+      <c r="A3" s="48"/>
       <c r="B3" s="20">
         <v>43865</v>
       </c>
       <c r="C3" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="59"/>
-      <c r="E3" s="55"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="64"/>
       <c r="F3" s="7"/>
       <c r="G3" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="H3" s="62"/>
-      <c r="I3" s="57"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="60"/>
       <c r="J3" s="7"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="52"/>
+      <c r="A4" s="48"/>
       <c r="B4" s="20">
         <v>43866</v>
       </c>
       <c r="C4" s="10"/>
-      <c r="D4" s="59"/>
-      <c r="E4" s="55"/>
+      <c r="D4" s="93"/>
+      <c r="E4" s="64"/>
       <c r="F4" s="7"/>
       <c r="G4" s="10"/>
-      <c r="H4" s="62"/>
-      <c r="I4" s="57"/>
+      <c r="H4" s="72"/>
+      <c r="I4" s="60"/>
       <c r="J4" s="7"/>
-      <c r="L4" s="42" t="s">
+      <c r="L4" s="83" t="s">
         <v>15</v>
       </c>
-      <c r="M4" s="43"/>
-      <c r="N4" s="43"/>
-      <c r="O4" s="44"/>
+      <c r="M4" s="84"/>
+      <c r="N4" s="84"/>
+      <c r="O4" s="85"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="52"/>
+      <c r="A5" s="48"/>
       <c r="B5" s="20">
         <v>43867</v>
       </c>
       <c r="C5" s="10"/>
-      <c r="D5" s="59"/>
-      <c r="E5" s="55"/>
+      <c r="D5" s="93"/>
+      <c r="E5" s="64"/>
       <c r="F5" s="7"/>
       <c r="G5" s="10"/>
-      <c r="H5" s="62"/>
-      <c r="I5" s="57"/>
+      <c r="H5" s="72"/>
+      <c r="I5" s="60"/>
       <c r="J5" s="7"/>
-      <c r="L5" s="45"/>
-      <c r="M5" s="46"/>
-      <c r="N5" s="46"/>
-      <c r="O5" s="47"/>
+      <c r="L5" s="86"/>
+      <c r="M5" s="87"/>
+      <c r="N5" s="87"/>
+      <c r="O5" s="88"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="52"/>
+      <c r="A6" s="48"/>
       <c r="B6" s="17">
         <v>43868</v>
       </c>
       <c r="C6" s="10"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="55"/>
+      <c r="D6" s="93"/>
+      <c r="E6" s="64"/>
       <c r="F6" s="7"/>
       <c r="G6" s="10"/>
-      <c r="H6" s="62"/>
-      <c r="I6" s="57"/>
+      <c r="H6" s="72"/>
+      <c r="I6" s="60"/>
       <c r="J6" s="7"/>
-      <c r="L6" s="45"/>
-      <c r="M6" s="46"/>
-      <c r="N6" s="46"/>
-      <c r="O6" s="47"/>
+      <c r="L6" s="86"/>
+      <c r="M6" s="87"/>
+      <c r="N6" s="87"/>
+      <c r="O6" s="88"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="52"/>
+      <c r="A7" s="48"/>
       <c r="B7" s="17">
         <v>43869</v>
       </c>
       <c r="C7" s="10"/>
-      <c r="D7" s="59"/>
-      <c r="E7" s="55"/>
+      <c r="D7" s="93"/>
+      <c r="E7" s="64"/>
       <c r="F7" s="7"/>
       <c r="G7" s="10"/>
-      <c r="H7" s="62"/>
-      <c r="I7" s="57"/>
+      <c r="H7" s="72"/>
+      <c r="I7" s="60"/>
       <c r="J7" s="7"/>
-      <c r="L7" s="45"/>
-      <c r="M7" s="46"/>
-      <c r="N7" s="46"/>
-      <c r="O7" s="47"/>
+      <c r="L7" s="86"/>
+      <c r="M7" s="87"/>
+      <c r="N7" s="87"/>
+      <c r="O7" s="88"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="53"/>
+      <c r="A8" s="49"/>
       <c r="B8" s="18">
         <v>43870</v>
       </c>
       <c r="C8" s="11"/>
-      <c r="D8" s="60"/>
-      <c r="E8" s="55"/>
+      <c r="D8" s="94"/>
+      <c r="E8" s="64"/>
       <c r="F8" s="7"/>
       <c r="G8" s="11"/>
-      <c r="H8" s="63"/>
-      <c r="I8" s="57"/>
+      <c r="H8" s="73"/>
+      <c r="I8" s="60"/>
       <c r="J8" s="7"/>
-      <c r="L8" s="45"/>
-      <c r="M8" s="46"/>
-      <c r="N8" s="46"/>
-      <c r="O8" s="47"/>
+      <c r="L8" s="86"/>
+      <c r="M8" s="87"/>
+      <c r="N8" s="87"/>
+      <c r="O8" s="88"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="51" t="s">
+      <c r="A9" s="47" t="s">
         <v>3</v>
       </c>
       <c r="B9" s="16">
@@ -1388,1199 +1383,1201 @@
       <c r="C9" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="79"/>
-      <c r="E9" s="56" t="s">
+      <c r="D9" s="65"/>
+      <c r="E9" s="59" t="s">
         <v>44</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="H9" s="82"/>
-      <c r="I9" s="56" t="s">
+      <c r="H9" s="68"/>
+      <c r="I9" s="59" t="s">
         <v>42</v>
       </c>
       <c r="J9" s="7"/>
-      <c r="L9" s="48"/>
-      <c r="M9" s="49"/>
-      <c r="N9" s="49"/>
-      <c r="O9" s="50"/>
+      <c r="L9" s="89"/>
+      <c r="M9" s="90"/>
+      <c r="N9" s="90"/>
+      <c r="O9" s="91"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="52"/>
+      <c r="A10" s="48"/>
       <c r="B10" s="17">
         <v>43872</v>
       </c>
       <c r="C10" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="80"/>
-      <c r="E10" s="57"/>
+      <c r="D10" s="66"/>
+      <c r="E10" s="60"/>
       <c r="F10" s="7"/>
       <c r="G10" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="H10" s="83"/>
-      <c r="I10" s="57"/>
+      <c r="H10" s="69"/>
+      <c r="I10" s="60"/>
       <c r="J10" s="7"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="52"/>
+      <c r="A11" s="48"/>
       <c r="B11" s="17">
         <v>43873</v>
       </c>
       <c r="C11" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="80"/>
-      <c r="E11" s="57"/>
+      <c r="D11" s="66"/>
+      <c r="E11" s="60"/>
       <c r="F11" s="7"/>
-      <c r="G11" s="28" t="s">
+      <c r="G11" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="H11" s="83"/>
-      <c r="I11" s="57"/>
+      <c r="H11" s="69"/>
+      <c r="I11" s="60"/>
       <c r="J11" s="7"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="52"/>
+      <c r="A12" s="48"/>
       <c r="B12" s="17">
         <v>43874</v>
       </c>
       <c r="C12" s="13"/>
-      <c r="D12" s="80"/>
-      <c r="E12" s="57"/>
+      <c r="D12" s="66"/>
+      <c r="E12" s="60"/>
       <c r="F12" s="7"/>
       <c r="G12" s="13"/>
-      <c r="H12" s="83"/>
-      <c r="I12" s="57"/>
+      <c r="H12" s="69"/>
+      <c r="I12" s="60"/>
       <c r="J12" s="7"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="52"/>
+      <c r="A13" s="48"/>
       <c r="B13" s="17">
         <v>43875</v>
       </c>
       <c r="C13" s="13"/>
-      <c r="D13" s="80"/>
-      <c r="E13" s="57"/>
+      <c r="D13" s="66"/>
+      <c r="E13" s="60"/>
       <c r="F13" s="7"/>
       <c r="G13" s="13"/>
-      <c r="H13" s="83"/>
-      <c r="I13" s="57"/>
+      <c r="H13" s="69"/>
+      <c r="I13" s="60"/>
       <c r="J13" s="7"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="52"/>
+      <c r="A14" s="48"/>
       <c r="B14" s="17">
         <v>43876</v>
       </c>
       <c r="C14" s="13"/>
-      <c r="D14" s="80"/>
-      <c r="E14" s="57"/>
+      <c r="D14" s="66"/>
+      <c r="E14" s="60"/>
       <c r="F14" s="7"/>
       <c r="G14" s="13"/>
-      <c r="H14" s="83"/>
-      <c r="I14" s="57"/>
+      <c r="H14" s="69"/>
+      <c r="I14" s="60"/>
       <c r="J14" s="7"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="53"/>
+      <c r="A15" s="49"/>
       <c r="B15" s="18">
         <v>43877</v>
       </c>
       <c r="C15" s="14"/>
-      <c r="D15" s="81"/>
-      <c r="E15" s="57"/>
+      <c r="D15" s="67"/>
+      <c r="E15" s="60"/>
       <c r="F15" s="7"/>
       <c r="G15" s="14"/>
-      <c r="H15" s="84"/>
-      <c r="I15" s="57"/>
+      <c r="H15" s="70"/>
+      <c r="I15" s="60"/>
       <c r="J15" s="7"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="51" t="s">
+      <c r="A16" s="47" t="s">
         <v>4</v>
       </c>
       <c r="B16" s="16">
         <v>43878</v>
       </c>
-      <c r="C16" s="30" t="s">
+      <c r="C16" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="79"/>
-      <c r="E16" s="56" t="s">
+      <c r="D16" s="65"/>
+      <c r="E16" s="59" t="s">
         <v>46</v>
       </c>
       <c r="F16" s="7"/>
-      <c r="G16" s="32" t="s">
+      <c r="G16" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="H16" s="71"/>
-      <c r="I16" s="54" t="s">
+      <c r="H16" s="82"/>
+      <c r="I16" s="78" t="s">
         <v>45</v>
       </c>
       <c r="J16" s="7"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="52"/>
+      <c r="A17" s="48"/>
       <c r="B17" s="17">
         <v>43879</v>
       </c>
       <c r="C17" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="80"/>
-      <c r="E17" s="57"/>
+      <c r="D17" s="66"/>
+      <c r="E17" s="60"/>
       <c r="F17" s="7"/>
-      <c r="G17" s="31" t="s">
+      <c r="G17" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="H17" s="69"/>
-      <c r="I17" s="55"/>
+      <c r="H17" s="80"/>
+      <c r="I17" s="64"/>
       <c r="J17" s="7"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="52"/>
+      <c r="A18" s="48"/>
       <c r="B18" s="17">
         <v>43880</v>
       </c>
       <c r="C18" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="80"/>
-      <c r="E18" s="57"/>
+      <c r="D18" s="66"/>
+      <c r="E18" s="60"/>
       <c r="F18" s="7"/>
       <c r="G18" s="22"/>
-      <c r="H18" s="69"/>
-      <c r="I18" s="55"/>
+      <c r="H18" s="80"/>
+      <c r="I18" s="64"/>
       <c r="J18" s="7"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="52"/>
+      <c r="A19" s="48"/>
       <c r="B19" s="17">
         <v>43881</v>
       </c>
-      <c r="C19" s="29" t="s">
+      <c r="C19" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="80"/>
-      <c r="E19" s="57"/>
+      <c r="D19" s="66"/>
+      <c r="E19" s="60"/>
       <c r="F19" s="7"/>
       <c r="G19" s="12"/>
-      <c r="H19" s="69"/>
-      <c r="I19" s="55"/>
+      <c r="H19" s="80"/>
+      <c r="I19" s="64"/>
       <c r="J19" s="7"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="52"/>
+      <c r="A20" s="48"/>
       <c r="B20" s="17">
         <v>43882</v>
       </c>
       <c r="C20" s="13"/>
-      <c r="D20" s="80"/>
-      <c r="E20" s="57"/>
+      <c r="D20" s="66"/>
+      <c r="E20" s="60"/>
       <c r="F20" s="7"/>
       <c r="G20" s="12"/>
-      <c r="H20" s="69"/>
-      <c r="I20" s="55"/>
+      <c r="H20" s="80"/>
+      <c r="I20" s="64"/>
       <c r="J20" s="7"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="52"/>
+      <c r="A21" s="48"/>
       <c r="B21" s="17">
         <v>43883</v>
       </c>
       <c r="C21" s="13"/>
-      <c r="D21" s="80"/>
-      <c r="E21" s="57"/>
+      <c r="D21" s="66"/>
+      <c r="E21" s="60"/>
       <c r="F21" s="7"/>
       <c r="G21" s="12"/>
-      <c r="H21" s="69"/>
-      <c r="I21" s="55"/>
+      <c r="H21" s="80"/>
+      <c r="I21" s="64"/>
       <c r="J21" s="7"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="53"/>
+      <c r="A22" s="49"/>
       <c r="B22" s="18">
         <v>43884</v>
       </c>
       <c r="C22" s="14"/>
-      <c r="D22" s="81"/>
-      <c r="E22" s="57"/>
+      <c r="D22" s="67"/>
+      <c r="E22" s="60"/>
       <c r="F22" s="7"/>
       <c r="G22" s="21"/>
-      <c r="H22" s="70"/>
-      <c r="I22" s="55"/>
+      <c r="H22" s="81"/>
+      <c r="I22" s="64"/>
       <c r="J22" s="7"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="51" t="s">
+      <c r="A23" s="47" t="s">
         <v>5</v>
       </c>
       <c r="B23" s="16">
         <v>43885</v>
       </c>
-      <c r="C23" s="33" t="s">
+      <c r="C23" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="58"/>
-      <c r="E23" s="54" t="s">
+      <c r="D23" s="92"/>
+      <c r="E23" s="78" t="s">
         <v>47</v>
       </c>
       <c r="F23" s="7"/>
-      <c r="G23" s="30" t="s">
+      <c r="G23" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="H23" s="68" t="s">
+      <c r="H23" s="79" t="s">
         <v>38</v>
       </c>
-      <c r="I23" s="54" t="s">
+      <c r="I23" s="78" t="s">
         <v>48</v>
       </c>
       <c r="J23" s="7"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="52"/>
+      <c r="A24" s="48"/>
       <c r="B24" s="17">
         <v>43886</v>
       </c>
       <c r="C24" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="D24" s="59"/>
-      <c r="E24" s="55"/>
+      <c r="D24" s="93"/>
+      <c r="E24" s="64"/>
       <c r="F24" s="7"/>
       <c r="G24" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="H24" s="69"/>
-      <c r="I24" s="55"/>
+      <c r="H24" s="80"/>
+      <c r="I24" s="64"/>
       <c r="J24" s="7"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="52"/>
+      <c r="A25" s="48"/>
       <c r="B25" s="17">
         <v>43887</v>
       </c>
       <c r="C25" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="D25" s="59"/>
-      <c r="E25" s="55"/>
+      <c r="D25" s="93"/>
+      <c r="E25" s="64"/>
       <c r="F25" s="7"/>
       <c r="G25" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="H25" s="69"/>
-      <c r="I25" s="55"/>
+      <c r="H25" s="80"/>
+      <c r="I25" s="64"/>
       <c r="J25" s="7"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="52"/>
+      <c r="A26" s="48"/>
       <c r="B26" s="17">
         <v>43888</v>
       </c>
-      <c r="C26" s="34" t="s">
+      <c r="C26" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="59"/>
-      <c r="E26" s="55"/>
+      <c r="D26" s="93"/>
+      <c r="E26" s="64"/>
       <c r="F26" s="7"/>
       <c r="G26" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="H26" s="69"/>
-      <c r="I26" s="55"/>
+      <c r="H26" s="80"/>
+      <c r="I26" s="64"/>
       <c r="J26" s="7"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="52"/>
+      <c r="A27" s="48"/>
       <c r="B27" s="17">
         <v>43889</v>
       </c>
-      <c r="C27" s="29" t="s">
+      <c r="C27" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="D27" s="59"/>
-      <c r="E27" s="55"/>
+      <c r="D27" s="93"/>
+      <c r="E27" s="64"/>
       <c r="F27" s="7"/>
       <c r="G27" s="13"/>
-      <c r="H27" s="69"/>
-      <c r="I27" s="55"/>
+      <c r="H27" s="80"/>
+      <c r="I27" s="64"/>
       <c r="J27" s="7"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="52"/>
+      <c r="A28" s="48"/>
       <c r="B28" s="17">
         <v>43890</v>
       </c>
       <c r="C28" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="D28" s="59"/>
-      <c r="E28" s="55"/>
+      <c r="D28" s="93"/>
+      <c r="E28" s="64"/>
       <c r="F28" s="7"/>
       <c r="G28" s="10"/>
-      <c r="H28" s="69"/>
-      <c r="I28" s="55"/>
+      <c r="H28" s="80"/>
+      <c r="I28" s="64"/>
       <c r="J28" s="7"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="53"/>
+      <c r="A29" s="49"/>
       <c r="B29" s="18">
         <v>43891</v>
       </c>
       <c r="C29" s="14"/>
-      <c r="D29" s="60"/>
-      <c r="E29" s="55"/>
+      <c r="D29" s="94"/>
+      <c r="E29" s="64"/>
       <c r="F29" s="7"/>
       <c r="G29" s="11"/>
-      <c r="H29" s="70"/>
-      <c r="I29" s="55"/>
+      <c r="H29" s="81"/>
+      <c r="I29" s="64"/>
       <c r="J29" s="7"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="51" t="s">
+      <c r="A30" s="47" t="s">
         <v>6</v>
       </c>
       <c r="B30" s="16">
         <v>43892</v>
       </c>
-      <c r="C30" s="29" t="s">
+      <c r="C30" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="D30" s="72"/>
-      <c r="E30" s="54" t="s">
+      <c r="D30" s="61"/>
+      <c r="E30" s="78" t="s">
         <v>51</v>
       </c>
       <c r="F30" s="7"/>
-      <c r="G30" s="30" t="s">
+      <c r="G30" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="H30" s="72"/>
-      <c r="I30" s="56" t="s">
+      <c r="H30" s="61"/>
+      <c r="I30" s="59" t="s">
         <v>50</v>
       </c>
       <c r="J30" s="7"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="52"/>
-      <c r="B31" s="35">
+      <c r="A31" s="48"/>
+      <c r="B31" s="34">
         <v>43893</v>
       </c>
-      <c r="C31" s="36" t="s">
+      <c r="C31" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="D31" s="78"/>
-      <c r="E31" s="55"/>
+      <c r="D31" s="57"/>
+      <c r="E31" s="64"/>
       <c r="F31" s="7"/>
       <c r="G31" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="H31" s="73"/>
-      <c r="I31" s="55"/>
+      <c r="H31" s="62"/>
+      <c r="I31" s="64"/>
       <c r="J31" s="7"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="52"/>
+      <c r="A32" s="48"/>
       <c r="B32" s="17">
         <v>43894</v>
       </c>
-      <c r="C32" s="36" t="s">
+      <c r="C32" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="D32" s="73"/>
-      <c r="E32" s="55"/>
+      <c r="D32" s="62"/>
+      <c r="E32" s="64"/>
       <c r="F32" s="7"/>
-      <c r="G32" s="36" t="s">
+      <c r="G32" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="H32" s="73"/>
-      <c r="I32" s="55"/>
+      <c r="H32" s="62"/>
+      <c r="I32" s="64"/>
       <c r="J32" s="7"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="52"/>
+      <c r="A33" s="48"/>
       <c r="B33" s="17">
         <v>43895</v>
       </c>
       <c r="C33" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="D33" s="73"/>
-      <c r="E33" s="55"/>
+      <c r="D33" s="62"/>
+      <c r="E33" s="64"/>
       <c r="F33" s="7"/>
-      <c r="G33" s="36" t="s">
+      <c r="G33" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="H33" s="73"/>
-      <c r="I33" s="55"/>
+      <c r="H33" s="62"/>
+      <c r="I33" s="64"/>
       <c r="J33" s="7"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="52"/>
+      <c r="A34" s="48"/>
       <c r="B34" s="17">
         <v>43896</v>
       </c>
-      <c r="C34" s="36" t="s">
+      <c r="C34" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="D34" s="73"/>
-      <c r="E34" s="55"/>
+      <c r="D34" s="62"/>
+      <c r="E34" s="64"/>
       <c r="F34" s="7"/>
       <c r="G34" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="H34" s="73"/>
-      <c r="I34" s="55"/>
+      <c r="H34" s="62"/>
+      <c r="I34" s="64"/>
       <c r="J34" s="7"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="52"/>
+      <c r="A35" s="48"/>
       <c r="B35" s="17">
         <v>43897</v>
       </c>
-      <c r="C35" s="36" t="s">
+      <c r="C35" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="D35" s="73"/>
-      <c r="E35" s="55"/>
+      <c r="D35" s="62"/>
+      <c r="E35" s="64"/>
       <c r="F35" s="7"/>
-      <c r="G35" s="10"/>
-      <c r="H35" s="73"/>
-      <c r="I35" s="55"/>
+      <c r="G35" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="H35" s="62"/>
+      <c r="I35" s="64"/>
       <c r="J35" s="7"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="53"/>
+      <c r="A36" s="49"/>
       <c r="B36" s="18">
         <v>43898</v>
       </c>
-      <c r="C36" s="37" t="s">
+      <c r="C36" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="D36" s="74"/>
-      <c r="E36" s="55"/>
+      <c r="D36" s="63"/>
+      <c r="E36" s="64"/>
       <c r="F36" s="7"/>
       <c r="G36" s="11"/>
-      <c r="H36" s="74"/>
-      <c r="I36" s="55"/>
+      <c r="H36" s="63"/>
+      <c r="I36" s="64"/>
       <c r="J36" s="7"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="51" t="s">
+      <c r="A37" s="47" t="s">
         <v>7</v>
       </c>
       <c r="B37" s="16">
         <v>43899</v>
       </c>
-      <c r="C37" s="29" t="s">
+      <c r="C37" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="D37" s="72"/>
-      <c r="E37" s="56" t="s">
+      <c r="D37" s="61"/>
+      <c r="E37" s="59" t="s">
         <v>52</v>
       </c>
       <c r="F37" s="7"/>
-      <c r="G37" s="30" t="s">
+      <c r="G37" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="H37" s="72"/>
-      <c r="I37" s="56" t="s">
+      <c r="H37" s="61"/>
+      <c r="I37" s="59" t="s">
         <v>53</v>
       </c>
       <c r="J37" s="7"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="52"/>
+      <c r="A38" s="48"/>
       <c r="B38" s="17">
         <v>43900</v>
       </c>
-      <c r="C38" s="39" t="s">
+      <c r="C38" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="D38" s="73"/>
-      <c r="E38" s="57"/>
+      <c r="D38" s="62"/>
+      <c r="E38" s="60"/>
       <c r="F38" s="7"/>
       <c r="G38" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="H38" s="73"/>
-      <c r="I38" s="55"/>
+      <c r="H38" s="62"/>
+      <c r="I38" s="64"/>
       <c r="J38" s="7"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="52"/>
+      <c r="A39" s="48"/>
       <c r="B39" s="17">
         <v>43901</v>
       </c>
-      <c r="C39" s="36" t="s">
+      <c r="C39" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="D39" s="73"/>
-      <c r="E39" s="57"/>
+      <c r="D39" s="62"/>
+      <c r="E39" s="60"/>
       <c r="F39" s="7"/>
       <c r="G39" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="H39" s="73"/>
-      <c r="I39" s="55"/>
+      <c r="H39" s="62"/>
+      <c r="I39" s="64"/>
       <c r="J39" s="7"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="52"/>
+      <c r="A40" s="48"/>
       <c r="B40" s="17">
         <v>43902</v>
       </c>
-      <c r="C40" s="30" t="s">
+      <c r="C40" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="D40" s="73"/>
-      <c r="E40" s="57"/>
+      <c r="D40" s="62"/>
+      <c r="E40" s="60"/>
       <c r="F40" s="7"/>
-      <c r="G40" s="38" t="s">
+      <c r="G40" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="H40" s="73"/>
-      <c r="I40" s="55"/>
+      <c r="H40" s="62"/>
+      <c r="I40" s="64"/>
       <c r="J40" s="7"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="52"/>
+      <c r="A41" s="48"/>
       <c r="B41" s="17">
         <v>43903</v>
       </c>
       <c r="C41" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="D41" s="73"/>
-      <c r="E41" s="57"/>
+      <c r="D41" s="62"/>
+      <c r="E41" s="60"/>
       <c r="F41" s="7"/>
       <c r="G41" s="13"/>
-      <c r="H41" s="73"/>
-      <c r="I41" s="55"/>
+      <c r="H41" s="62"/>
+      <c r="I41" s="64"/>
       <c r="J41" s="7"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="52"/>
+      <c r="A42" s="48"/>
       <c r="B42" s="17">
         <v>43904</v>
       </c>
-      <c r="C42" s="36" t="s">
+      <c r="C42" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="D42" s="73"/>
-      <c r="E42" s="57"/>
+      <c r="D42" s="62"/>
+      <c r="E42" s="60"/>
       <c r="F42" s="7"/>
       <c r="G42" s="13"/>
-      <c r="H42" s="73"/>
-      <c r="I42" s="55"/>
+      <c r="H42" s="62"/>
+      <c r="I42" s="64"/>
       <c r="J42" s="7"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="53"/>
+      <c r="A43" s="49"/>
       <c r="B43" s="18">
         <v>43905</v>
       </c>
-      <c r="C43" s="40" t="s">
+      <c r="C43" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="D43" s="74"/>
-      <c r="E43" s="57"/>
+      <c r="D43" s="63"/>
+      <c r="E43" s="60"/>
       <c r="F43" s="7"/>
       <c r="G43" s="13"/>
-      <c r="H43" s="74"/>
-      <c r="I43" s="55"/>
+      <c r="H43" s="63"/>
+      <c r="I43" s="64"/>
       <c r="J43" s="7"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="51" t="s">
+      <c r="A44" s="47" t="s">
         <v>8</v>
       </c>
       <c r="B44" s="18">
         <v>43906</v>
       </c>
-      <c r="C44" s="36" t="s">
+      <c r="C44" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="D44" s="72"/>
-      <c r="E44" s="56" t="s">
+      <c r="D44" s="61"/>
+      <c r="E44" s="59" t="s">
         <v>55</v>
       </c>
       <c r="F44" s="7"/>
-      <c r="G44" s="29" t="s">
+      <c r="G44" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="H44" s="85"/>
-      <c r="I44" s="56" t="s">
+      <c r="H44" s="56"/>
+      <c r="I44" s="59" t="s">
         <v>61</v>
       </c>
       <c r="J44" s="7"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="52"/>
+      <c r="A45" s="48"/>
       <c r="B45" s="18">
         <v>43907</v>
       </c>
       <c r="C45" s="13"/>
-      <c r="D45" s="73"/>
-      <c r="E45" s="57"/>
+      <c r="D45" s="62"/>
+      <c r="E45" s="60"/>
       <c r="F45" s="7"/>
-      <c r="G45" s="36" t="s">
+      <c r="G45" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="H45" s="78"/>
-      <c r="I45" s="55"/>
+      <c r="H45" s="57"/>
+      <c r="I45" s="64"/>
       <c r="J45" s="7"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="52"/>
+      <c r="A46" s="48"/>
       <c r="B46" s="18">
         <v>43908</v>
       </c>
       <c r="C46" s="13"/>
-      <c r="D46" s="73"/>
-      <c r="E46" s="57"/>
+      <c r="D46" s="62"/>
+      <c r="E46" s="60"/>
       <c r="F46" s="7"/>
       <c r="G46" s="13"/>
-      <c r="H46" s="78"/>
-      <c r="I46" s="55"/>
+      <c r="H46" s="57"/>
+      <c r="I46" s="64"/>
       <c r="J46" s="7"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="52"/>
+      <c r="A47" s="48"/>
       <c r="B47" s="18">
         <v>43909</v>
       </c>
       <c r="C47" s="13"/>
-      <c r="D47" s="73"/>
-      <c r="E47" s="57"/>
+      <c r="D47" s="62"/>
+      <c r="E47" s="60"/>
       <c r="F47" s="7"/>
       <c r="G47" s="13"/>
-      <c r="H47" s="78"/>
-      <c r="I47" s="55"/>
+      <c r="H47" s="57"/>
+      <c r="I47" s="64"/>
       <c r="J47" s="7"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="52"/>
+      <c r="A48" s="48"/>
       <c r="B48" s="18">
         <v>43910</v>
       </c>
       <c r="C48" s="13"/>
-      <c r="D48" s="73"/>
-      <c r="E48" s="57"/>
+      <c r="D48" s="62"/>
+      <c r="E48" s="60"/>
       <c r="F48" s="7"/>
       <c r="G48" s="13"/>
-      <c r="H48" s="78"/>
-      <c r="I48" s="55"/>
+      <c r="H48" s="57"/>
+      <c r="I48" s="64"/>
       <c r="J48" s="7"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="52"/>
+      <c r="A49" s="48"/>
       <c r="B49" s="18">
         <v>43911</v>
       </c>
       <c r="C49" s="13"/>
-      <c r="D49" s="73"/>
-      <c r="E49" s="57"/>
+      <c r="D49" s="62"/>
+      <c r="E49" s="60"/>
       <c r="F49" s="7"/>
       <c r="G49" s="13"/>
-      <c r="H49" s="78"/>
-      <c r="I49" s="55"/>
+      <c r="H49" s="57"/>
+      <c r="I49" s="64"/>
       <c r="J49" s="7"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="53"/>
+      <c r="A50" s="49"/>
       <c r="B50" s="18">
         <v>43912</v>
       </c>
       <c r="C50" s="14"/>
-      <c r="D50" s="74"/>
-      <c r="E50" s="57"/>
+      <c r="D50" s="63"/>
+      <c r="E50" s="60"/>
       <c r="F50" s="7"/>
       <c r="G50" s="14"/>
-      <c r="H50" s="86"/>
-      <c r="I50" s="55"/>
+      <c r="H50" s="58"/>
+      <c r="I50" s="64"/>
       <c r="J50" s="7"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" s="51" t="s">
+      <c r="A51" s="47" t="s">
         <v>57</v>
       </c>
       <c r="B51" s="18">
         <v>43913</v>
       </c>
-      <c r="C51" s="29" t="s">
+      <c r="C51" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="D51" s="72"/>
-      <c r="E51" s="56" t="s">
+      <c r="D51" s="61"/>
+      <c r="E51" s="59" t="s">
         <v>40</v>
       </c>
       <c r="F51" s="7"/>
-      <c r="G51" s="29" t="s">
+      <c r="G51" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="H51" s="85"/>
-      <c r="I51" s="56" t="s">
+      <c r="H51" s="56"/>
+      <c r="I51" s="59" t="s">
         <v>68</v>
       </c>
       <c r="J51" s="7"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="52"/>
+      <c r="A52" s="48"/>
       <c r="B52" s="18">
         <v>43914</v>
       </c>
-      <c r="C52" s="36" t="s">
+      <c r="C52" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="D52" s="73"/>
-      <c r="E52" s="57"/>
+      <c r="D52" s="62"/>
+      <c r="E52" s="60"/>
       <c r="F52" s="7"/>
       <c r="G52" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="H52" s="78"/>
-      <c r="I52" s="57"/>
+      <c r="H52" s="57"/>
+      <c r="I52" s="60"/>
       <c r="J52" s="7"/>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" s="52"/>
+      <c r="A53" s="48"/>
       <c r="B53" s="18">
         <v>43915</v>
       </c>
-      <c r="C53" s="36" t="s">
+      <c r="C53" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="D53" s="73"/>
-      <c r="E53" s="57"/>
+      <c r="D53" s="62"/>
+      <c r="E53" s="60"/>
       <c r="F53" s="7"/>
       <c r="G53" s="13"/>
-      <c r="H53" s="78"/>
-      <c r="I53" s="57"/>
+      <c r="H53" s="57"/>
+      <c r="I53" s="60"/>
       <c r="J53" s="7"/>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A54" s="52"/>
+      <c r="A54" s="48"/>
       <c r="B54" s="18">
         <v>43916</v>
       </c>
-      <c r="C54" s="36" t="s">
+      <c r="C54" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="D54" s="73"/>
-      <c r="E54" s="57"/>
+      <c r="D54" s="62"/>
+      <c r="E54" s="60"/>
       <c r="F54" s="7"/>
       <c r="G54" s="13"/>
-      <c r="H54" s="78"/>
-      <c r="I54" s="57"/>
+      <c r="H54" s="57"/>
+      <c r="I54" s="60"/>
       <c r="J54" s="7"/>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" s="52"/>
+      <c r="A55" s="48"/>
       <c r="B55" s="18">
         <v>43917</v>
       </c>
       <c r="C55" s="13"/>
-      <c r="D55" s="73"/>
-      <c r="E55" s="57"/>
+      <c r="D55" s="62"/>
+      <c r="E55" s="60"/>
       <c r="F55" s="7"/>
       <c r="G55" s="13"/>
-      <c r="H55" s="78"/>
-      <c r="I55" s="57"/>
+      <c r="H55" s="57"/>
+      <c r="I55" s="60"/>
       <c r="J55" s="7"/>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56" s="52"/>
+      <c r="A56" s="48"/>
       <c r="B56" s="18">
         <v>43918</v>
       </c>
       <c r="C56" s="13"/>
-      <c r="D56" s="73"/>
-      <c r="E56" s="57"/>
+      <c r="D56" s="62"/>
+      <c r="E56" s="60"/>
       <c r="F56" s="7"/>
       <c r="G56" s="13"/>
-      <c r="H56" s="78"/>
-      <c r="I56" s="57"/>
+      <c r="H56" s="57"/>
+      <c r="I56" s="60"/>
       <c r="J56" s="7"/>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A57" s="53"/>
+      <c r="A57" s="49"/>
       <c r="B57" s="18">
         <v>43919</v>
       </c>
       <c r="C57" s="13"/>
-      <c r="D57" s="74"/>
-      <c r="E57" s="57"/>
+      <c r="D57" s="63"/>
+      <c r="E57" s="60"/>
       <c r="F57" s="7"/>
       <c r="G57" s="13"/>
-      <c r="H57" s="86"/>
-      <c r="I57" s="57"/>
+      <c r="H57" s="58"/>
+      <c r="I57" s="60"/>
       <c r="J57" s="7"/>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A58" s="51" t="s">
+      <c r="A58" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="B58" s="41">
+      <c r="B58" s="40">
         <v>43920</v>
       </c>
-      <c r="C58" s="29" t="s">
+      <c r="C58" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="D58" s="85"/>
-      <c r="E58" s="56" t="s">
+      <c r="D58" s="56"/>
+      <c r="E58" s="59" t="s">
         <v>40</v>
       </c>
       <c r="F58" s="7"/>
-      <c r="G58" s="29" t="s">
+      <c r="G58" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="H58" s="85"/>
-      <c r="I58" s="56" t="s">
+      <c r="H58" s="56"/>
+      <c r="I58" s="59" t="s">
         <v>40</v>
       </c>
       <c r="J58" s="7"/>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A59" s="52"/>
-      <c r="B59" s="41">
+      <c r="A59" s="48"/>
+      <c r="B59" s="40">
         <v>43921</v>
       </c>
-      <c r="C59" s="36" t="s">
+      <c r="C59" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="D59" s="78"/>
-      <c r="E59" s="57"/>
+      <c r="D59" s="57"/>
+      <c r="E59" s="60"/>
       <c r="F59" s="7"/>
-      <c r="G59" s="29" t="s">
+      <c r="G59" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="H59" s="78"/>
-      <c r="I59" s="57"/>
+      <c r="H59" s="57"/>
+      <c r="I59" s="60"/>
       <c r="J59" s="7"/>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A60" s="52"/>
-      <c r="B60" s="41">
+      <c r="A60" s="48"/>
+      <c r="B60" s="40">
         <v>43922</v>
       </c>
-      <c r="C60" s="36" t="s">
+      <c r="C60" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="D60" s="78"/>
-      <c r="E60" s="57"/>
+      <c r="D60" s="57"/>
+      <c r="E60" s="60"/>
       <c r="F60" s="7"/>
       <c r="G60" s="13"/>
-      <c r="H60" s="78"/>
-      <c r="I60" s="57"/>
+      <c r="H60" s="57"/>
+      <c r="I60" s="60"/>
       <c r="J60" s="7"/>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A61" s="52"/>
-      <c r="B61" s="41">
+      <c r="A61" s="48"/>
+      <c r="B61" s="40">
         <v>43923</v>
       </c>
-      <c r="C61" s="36" t="s">
+      <c r="C61" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="D61" s="78"/>
-      <c r="E61" s="57"/>
+      <c r="D61" s="57"/>
+      <c r="E61" s="60"/>
       <c r="F61" s="7"/>
       <c r="G61" s="13"/>
-      <c r="H61" s="78"/>
-      <c r="I61" s="57"/>
+      <c r="H61" s="57"/>
+      <c r="I61" s="60"/>
       <c r="J61" s="7"/>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A62" s="52"/>
-      <c r="B62" s="41">
+      <c r="A62" s="48"/>
+      <c r="B62" s="40">
         <v>43924</v>
       </c>
       <c r="C62" s="13"/>
-      <c r="D62" s="78"/>
-      <c r="E62" s="57"/>
+      <c r="D62" s="57"/>
+      <c r="E62" s="60"/>
       <c r="F62" s="7"/>
       <c r="G62" s="13"/>
-      <c r="H62" s="78"/>
-      <c r="I62" s="57"/>
+      <c r="H62" s="57"/>
+      <c r="I62" s="60"/>
       <c r="J62" s="7"/>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A63" s="52"/>
-      <c r="B63" s="41">
+      <c r="A63" s="48"/>
+      <c r="B63" s="40">
         <v>43925</v>
       </c>
       <c r="C63" s="13"/>
-      <c r="D63" s="78"/>
-      <c r="E63" s="57"/>
+      <c r="D63" s="57"/>
+      <c r="E63" s="60"/>
       <c r="F63" s="7"/>
       <c r="G63" s="13"/>
-      <c r="H63" s="78"/>
-      <c r="I63" s="57"/>
+      <c r="H63" s="57"/>
+      <c r="I63" s="60"/>
       <c r="J63" s="7"/>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A64" s="53"/>
-      <c r="B64" s="41">
+      <c r="A64" s="49"/>
+      <c r="B64" s="40">
         <v>43926</v>
       </c>
       <c r="C64" s="13"/>
-      <c r="D64" s="86"/>
-      <c r="E64" s="57"/>
+      <c r="D64" s="58"/>
+      <c r="E64" s="60"/>
       <c r="F64" s="7"/>
       <c r="G64" s="13"/>
-      <c r="H64" s="86"/>
-      <c r="I64" s="57"/>
+      <c r="H64" s="58"/>
+      <c r="I64" s="60"/>
       <c r="J64" s="7"/>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A65" s="51" t="s">
+      <c r="A65" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="B65" s="41">
+      <c r="B65" s="40">
         <v>43927</v>
       </c>
-      <c r="C65" s="29" t="s">
+      <c r="C65" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="D65" s="75"/>
-      <c r="E65" s="75" t="s">
+      <c r="D65" s="50"/>
+      <c r="E65" s="50" t="s">
         <v>67</v>
       </c>
       <c r="F65" s="7"/>
-      <c r="G65" s="29" t="s">
+      <c r="G65" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="H65" s="75"/>
-      <c r="I65" s="91" t="s">
+      <c r="H65" s="50"/>
+      <c r="I65" s="53" t="s">
         <v>70</v>
       </c>
       <c r="J65" s="7"/>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A66" s="52"/>
-      <c r="B66" s="41">
+      <c r="A66" s="48"/>
+      <c r="B66" s="40">
         <v>43928</v>
       </c>
-      <c r="C66" s="36" t="s">
+      <c r="C66" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="D66" s="76"/>
-      <c r="E66" s="76"/>
+      <c r="D66" s="51"/>
+      <c r="E66" s="51"/>
       <c r="F66" s="7"/>
-      <c r="G66" s="29" t="s">
+      <c r="G66" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="H66" s="76"/>
-      <c r="I66" s="76"/>
+      <c r="H66" s="51"/>
+      <c r="I66" s="51"/>
       <c r="J66" s="7"/>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A67" s="52"/>
-      <c r="B67" s="41">
+      <c r="A67" s="48"/>
+      <c r="B67" s="40">
         <v>43929</v>
       </c>
-      <c r="C67" s="36" t="s">
+      <c r="C67" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="D67" s="76"/>
-      <c r="E67" s="76"/>
+      <c r="D67" s="51"/>
+      <c r="E67" s="51"/>
       <c r="F67" s="7"/>
       <c r="G67" s="13"/>
-      <c r="H67" s="76"/>
-      <c r="I67" s="76"/>
+      <c r="H67" s="51"/>
+      <c r="I67" s="51"/>
       <c r="J67" s="7"/>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A68" s="52"/>
-      <c r="B68" s="41">
+      <c r="A68" s="48"/>
+      <c r="B68" s="40">
         <v>43930</v>
       </c>
-      <c r="C68" s="36" t="s">
+      <c r="C68" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="D68" s="76"/>
-      <c r="E68" s="76"/>
+      <c r="D68" s="51"/>
+      <c r="E68" s="51"/>
       <c r="F68" s="7"/>
       <c r="G68" s="13"/>
-      <c r="H68" s="76"/>
-      <c r="I68" s="76"/>
+      <c r="H68" s="51"/>
+      <c r="I68" s="51"/>
       <c r="J68" s="7"/>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A69" s="52"/>
-      <c r="B69" s="41">
+      <c r="A69" s="48"/>
+      <c r="B69" s="40">
         <v>43931</v>
       </c>
       <c r="C69" s="13"/>
-      <c r="D69" s="76"/>
-      <c r="E69" s="76"/>
+      <c r="D69" s="51"/>
+      <c r="E69" s="51"/>
       <c r="F69" s="7"/>
       <c r="G69" s="13"/>
-      <c r="H69" s="76"/>
-      <c r="I69" s="76"/>
+      <c r="H69" s="51"/>
+      <c r="I69" s="51"/>
       <c r="J69" s="7"/>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A70" s="52"/>
-      <c r="B70" s="41">
+      <c r="A70" s="48"/>
+      <c r="B70" s="40">
         <v>43932</v>
       </c>
       <c r="C70" s="13"/>
-      <c r="D70" s="76"/>
-      <c r="E70" s="76"/>
+      <c r="D70" s="51"/>
+      <c r="E70" s="51"/>
       <c r="F70" s="7"/>
       <c r="G70" s="13"/>
-      <c r="H70" s="76"/>
-      <c r="I70" s="76"/>
+      <c r="H70" s="51"/>
+      <c r="I70" s="51"/>
       <c r="J70" s="7"/>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A71" s="53"/>
-      <c r="B71" s="41">
+      <c r="A71" s="49"/>
+      <c r="B71" s="40">
         <v>43933</v>
       </c>
       <c r="C71" s="14"/>
-      <c r="D71" s="77"/>
-      <c r="E71" s="77"/>
+      <c r="D71" s="52"/>
+      <c r="E71" s="52"/>
       <c r="F71" s="7"/>
       <c r="G71" s="13"/>
-      <c r="H71" s="77"/>
-      <c r="I71" s="77"/>
+      <c r="H71" s="52"/>
+      <c r="I71" s="52"/>
       <c r="J71" s="7"/>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A72" s="51" t="s">
+      <c r="A72" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="B72" s="41">
+      <c r="B72" s="40">
         <v>43934</v>
       </c>
       <c r="C72" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="D72" s="75"/>
-      <c r="E72" s="75" t="s">
+      <c r="D72" s="50"/>
+      <c r="E72" s="50" t="s">
         <v>73</v>
       </c>
       <c r="F72" s="7"/>
       <c r="G72" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="H72" s="75"/>
-      <c r="I72" s="91" t="s">
+      <c r="H72" s="50"/>
+      <c r="I72" s="53" t="s">
         <v>74</v>
       </c>
       <c r="J72" s="7"/>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A73" s="52"/>
-      <c r="B73" s="41">
+      <c r="A73" s="48"/>
+      <c r="B73" s="40">
         <v>43935</v>
       </c>
-      <c r="C73" s="36" t="s">
+      <c r="C73" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="D73" s="76"/>
-      <c r="E73" s="76"/>
+      <c r="D73" s="51"/>
+      <c r="E73" s="51"/>
       <c r="F73" s="7"/>
-      <c r="G73" s="29" t="s">
+      <c r="G73" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="H73" s="76"/>
-      <c r="I73" s="92"/>
+      <c r="H73" s="51"/>
+      <c r="I73" s="54"/>
       <c r="J73" s="7"/>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A74" s="52"/>
-      <c r="B74" s="41">
+      <c r="A74" s="48"/>
+      <c r="B74" s="40">
         <v>43936</v>
       </c>
-      <c r="C74" s="36" t="s">
+      <c r="C74" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="D74" s="76"/>
-      <c r="E74" s="76"/>
+      <c r="D74" s="51"/>
+      <c r="E74" s="51"/>
       <c r="F74" s="7"/>
-      <c r="G74" s="38" t="s">
+      <c r="G74" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="H74" s="76"/>
-      <c r="I74" s="92"/>
+      <c r="H74" s="51"/>
+      <c r="I74" s="54"/>
       <c r="J74" s="7"/>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A75" s="52"/>
-      <c r="B75" s="41">
+      <c r="A75" s="48"/>
+      <c r="B75" s="40">
         <v>43937</v>
       </c>
       <c r="C75" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="D75" s="76"/>
-      <c r="E75" s="76"/>
+      <c r="D75" s="51"/>
+      <c r="E75" s="51"/>
       <c r="F75" s="7"/>
-      <c r="G75" s="30" t="s">
+      <c r="G75" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="H75" s="76"/>
-      <c r="I75" s="92"/>
+      <c r="H75" s="51"/>
+      <c r="I75" s="54"/>
       <c r="J75" s="7"/>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A76" s="52"/>
-      <c r="B76" s="41">
+      <c r="A76" s="48"/>
+      <c r="B76" s="40">
         <v>43938</v>
       </c>
       <c r="C76" s="13"/>
-      <c r="D76" s="76"/>
-      <c r="E76" s="76"/>
+      <c r="D76" s="51"/>
+      <c r="E76" s="51"/>
       <c r="F76" s="7"/>
       <c r="G76" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="H76" s="76"/>
-      <c r="I76" s="92"/>
+      <c r="H76" s="51"/>
+      <c r="I76" s="54"/>
       <c r="J76" s="7"/>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A77" s="52"/>
-      <c r="B77" s="41">
+      <c r="A77" s="48"/>
+      <c r="B77" s="40">
         <v>43939</v>
       </c>
       <c r="C77" s="13"/>
-      <c r="D77" s="76"/>
-      <c r="E77" s="76"/>
+      <c r="D77" s="51"/>
+      <c r="E77" s="51"/>
       <c r="F77" s="7"/>
       <c r="G77" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="H77" s="76"/>
-      <c r="I77" s="92"/>
+      <c r="H77" s="51"/>
+      <c r="I77" s="54"/>
       <c r="J77" s="7"/>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A78" s="53"/>
-      <c r="B78" s="41">
+      <c r="A78" s="49"/>
+      <c r="B78" s="40">
         <v>43940</v>
       </c>
       <c r="C78" s="14"/>
-      <c r="D78" s="77"/>
-      <c r="E78" s="77"/>
+      <c r="D78" s="52"/>
+      <c r="E78" s="52"/>
       <c r="F78" s="7"/>
       <c r="G78" s="13"/>
-      <c r="H78" s="77"/>
-      <c r="I78" s="93"/>
+      <c r="H78" s="52"/>
+      <c r="I78" s="55"/>
       <c r="J78" s="7"/>
     </row>
     <row r="79" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="51" t="s">
+      <c r="A79" s="47" t="s">
         <v>65</v>
       </c>
-      <c r="B79" s="41">
+      <c r="B79" s="40">
         <v>43941</v>
       </c>
       <c r="C79" s="24" t="s">
@@ -2589,7 +2586,7 @@
       <c r="D79" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E79" s="65"/>
+      <c r="E79" s="75"/>
       <c r="F79" s="7"/>
       <c r="G79" s="23" t="s">
         <v>56</v>
@@ -2597,12 +2594,12 @@
       <c r="H79" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="I79" s="66"/>
+      <c r="I79" s="76"/>
       <c r="J79" s="7"/>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A80" s="52"/>
-      <c r="B80" s="41">
+      <c r="A80" s="48"/>
+      <c r="B80" s="40">
         <v>43942</v>
       </c>
       <c r="C80" s="24" t="s">
@@ -2611,27 +2608,27 @@
       <c r="D80" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E80" s="65"/>
+      <c r="E80" s="75"/>
       <c r="F80" s="7"/>
-      <c r="G80" s="39" t="s">
+      <c r="G80" s="38" t="s">
         <v>43</v>
       </c>
       <c r="H80" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="I80" s="67"/>
+      <c r="I80" s="77"/>
       <c r="J80" s="7"/>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A81" s="52"/>
-      <c r="B81" s="41">
+      <c r="A81" s="48"/>
+      <c r="B81" s="40">
         <v>43943</v>
       </c>
-      <c r="C81" s="87"/>
+      <c r="C81" s="41"/>
       <c r="D81" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E81" s="65"/>
+      <c r="E81" s="75"/>
       <c r="F81" s="7"/>
       <c r="G81" s="24" t="s">
         <v>28</v>
@@ -2639,19 +2636,19 @@
       <c r="H81" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I81" s="67"/>
+      <c r="I81" s="77"/>
       <c r="J81" s="7"/>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A82" s="52"/>
-      <c r="B82" s="41">
+      <c r="A82" s="48"/>
+      <c r="B82" s="40">
         <v>43944</v>
       </c>
-      <c r="C82" s="87"/>
+      <c r="C82" s="41"/>
       <c r="D82" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E82" s="65"/>
+      <c r="E82" s="75"/>
       <c r="F82" s="7"/>
       <c r="G82" s="24" t="s">
         <v>32</v>
@@ -2659,55 +2656,55 @@
       <c r="H82" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I82" s="67"/>
+      <c r="I82" s="77"/>
       <c r="J82" s="7"/>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A83" s="52"/>
-      <c r="B83" s="41">
+      <c r="A83" s="48"/>
+      <c r="B83" s="40">
         <v>43945</v>
       </c>
-      <c r="C83" s="87"/>
+      <c r="C83" s="41"/>
       <c r="D83" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E83" s="65"/>
+      <c r="E83" s="75"/>
       <c r="F83" s="7"/>
-      <c r="G83" s="87"/>
+      <c r="G83" s="41"/>
       <c r="H83" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I83" s="67"/>
+      <c r="I83" s="77"/>
       <c r="J83" s="7"/>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A84" s="52"/>
-      <c r="B84" s="41">
+      <c r="A84" s="48"/>
+      <c r="B84" s="40">
         <v>43946</v>
       </c>
-      <c r="C84" s="87"/>
-      <c r="D84" s="94" t="s">
+      <c r="C84" s="41"/>
+      <c r="D84" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="E84" s="65"/>
+      <c r="E84" s="75"/>
       <c r="F84" s="7"/>
-      <c r="G84" s="89"/>
-      <c r="H84" s="95" t="s">
+      <c r="G84" s="43"/>
+      <c r="H84" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="I84" s="65"/>
+      <c r="I84" s="75"/>
       <c r="J84" s="7"/>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A85" s="53"/>
+      <c r="A85" s="49"/>
       <c r="B85" s="7"/>
-      <c r="C85" s="88"/>
+      <c r="C85" s="42"/>
       <c r="D85" s="7"/>
-      <c r="E85" s="65"/>
+      <c r="E85" s="75"/>
       <c r="F85" s="7"/>
-      <c r="G85" s="90"/>
+      <c r="G85" s="44"/>
       <c r="H85" s="15"/>
-      <c r="I85" s="65"/>
+      <c r="I85" s="75"/>
       <c r="J85" s="7"/>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
@@ -2724,35 +2721,21 @@
     </row>
   </sheetData>
   <mergeCells count="59">
-    <mergeCell ref="A72:A78"/>
-    <mergeCell ref="D72:D78"/>
-    <mergeCell ref="E72:E78"/>
-    <mergeCell ref="H72:H78"/>
-    <mergeCell ref="I72:I78"/>
-    <mergeCell ref="H58:H64"/>
-    <mergeCell ref="H65:H71"/>
-    <mergeCell ref="A58:A64"/>
-    <mergeCell ref="A65:A71"/>
-    <mergeCell ref="D58:D64"/>
-    <mergeCell ref="D65:D71"/>
-    <mergeCell ref="E58:E64"/>
-    <mergeCell ref="E65:E71"/>
-    <mergeCell ref="A51:A57"/>
-    <mergeCell ref="D51:D57"/>
-    <mergeCell ref="E51:E57"/>
-    <mergeCell ref="H51:H57"/>
-    <mergeCell ref="I51:I57"/>
-    <mergeCell ref="A44:A50"/>
-    <mergeCell ref="H44:H50"/>
-    <mergeCell ref="D44:D50"/>
-    <mergeCell ref="E44:E50"/>
-    <mergeCell ref="I44:I50"/>
-    <mergeCell ref="D30:D36"/>
-    <mergeCell ref="D37:D43"/>
-    <mergeCell ref="H37:H43"/>
-    <mergeCell ref="D9:D15"/>
-    <mergeCell ref="D16:D22"/>
-    <mergeCell ref="H9:H15"/>
+    <mergeCell ref="L4:O9"/>
+    <mergeCell ref="A30:A36"/>
+    <mergeCell ref="A37:A43"/>
+    <mergeCell ref="A79:A85"/>
+    <mergeCell ref="A9:A15"/>
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="A16:A22"/>
+    <mergeCell ref="A23:A29"/>
+    <mergeCell ref="E2:E8"/>
+    <mergeCell ref="E9:E15"/>
+    <mergeCell ref="E23:E29"/>
+    <mergeCell ref="E30:E36"/>
+    <mergeCell ref="E37:E43"/>
+    <mergeCell ref="D2:D8"/>
+    <mergeCell ref="D23:D29"/>
     <mergeCell ref="H2:H8"/>
     <mergeCell ref="I2:I8"/>
     <mergeCell ref="E79:E85"/>
@@ -2768,21 +2751,35 @@
     <mergeCell ref="H30:H36"/>
     <mergeCell ref="I58:I64"/>
     <mergeCell ref="I65:I71"/>
-    <mergeCell ref="L4:O9"/>
-    <mergeCell ref="A30:A36"/>
-    <mergeCell ref="A37:A43"/>
-    <mergeCell ref="A79:A85"/>
-    <mergeCell ref="A9:A15"/>
-    <mergeCell ref="A2:A8"/>
-    <mergeCell ref="A16:A22"/>
-    <mergeCell ref="A23:A29"/>
-    <mergeCell ref="E2:E8"/>
-    <mergeCell ref="E9:E15"/>
-    <mergeCell ref="E23:E29"/>
-    <mergeCell ref="E30:E36"/>
-    <mergeCell ref="E37:E43"/>
-    <mergeCell ref="D2:D8"/>
-    <mergeCell ref="D23:D29"/>
+    <mergeCell ref="D30:D36"/>
+    <mergeCell ref="D37:D43"/>
+    <mergeCell ref="H37:H43"/>
+    <mergeCell ref="D9:D15"/>
+    <mergeCell ref="D16:D22"/>
+    <mergeCell ref="H9:H15"/>
+    <mergeCell ref="A44:A50"/>
+    <mergeCell ref="H44:H50"/>
+    <mergeCell ref="D44:D50"/>
+    <mergeCell ref="E44:E50"/>
+    <mergeCell ref="I44:I50"/>
+    <mergeCell ref="A51:A57"/>
+    <mergeCell ref="D51:D57"/>
+    <mergeCell ref="E51:E57"/>
+    <mergeCell ref="H51:H57"/>
+    <mergeCell ref="I51:I57"/>
+    <mergeCell ref="H58:H64"/>
+    <mergeCell ref="H65:H71"/>
+    <mergeCell ref="A58:A64"/>
+    <mergeCell ref="A65:A71"/>
+    <mergeCell ref="D58:D64"/>
+    <mergeCell ref="D65:D71"/>
+    <mergeCell ref="E58:E64"/>
+    <mergeCell ref="E65:E71"/>
+    <mergeCell ref="A72:A78"/>
+    <mergeCell ref="D72:D78"/>
+    <mergeCell ref="E72:E78"/>
+    <mergeCell ref="H72:H78"/>
+    <mergeCell ref="I72:I78"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>